<commit_message>
Further updates to validation
</commit_message>
<xml_diff>
--- a/Excel LHDN Calculator Form (Blank Form).xlsx
+++ b/Excel LHDN Calculator Form (Blank Form).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harein\Documents\GitHub\MY_TaxRelief\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A34E86-B7A2-4F8E-ABEB-58685959C22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BBBCEE-D2A3-4EA7-81AD-EA7989F5A2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="777" activeTab="3" xr2:uid="{4EA980A6-4219-484D-BF26-8C30E1E17AF4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="777" xr2:uid="{4EA980A6-4219-484D-BF26-8C30E1E17AF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Compute Income Tax (Part B)" sheetId="1" r:id="rId1"/>
@@ -4494,10 +4494,10 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B2" sqref="B2:B44"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51:C57"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5445,8 +5445,8 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5957,9 +5957,9 @@
   <dimension ref="A1:E225"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B2" sqref="B2:B44"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7:D8"/>
+      <selection pane="bottomLeft" activeCell="D228" sqref="D228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8413,7 +8413,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="901" yWindow="454" count="35">
+  <dataValidations xWindow="901" yWindow="454" count="36">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J15" xr:uid="{7C5F2CC9-69A1-48F9-827C-64E5131B3870}">
       <formula1>_xlfn.FORMULATEXT(J15)</formula1>
     </dataValidation>
@@ -8433,7 +8433,7 @@
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Data, Number or Ineligible" error="The input data or number is invalid, or you may be ineligible to claim this relief. _x000a__x000a_Note that if you claimed the relief of Item F14b(ii), you are not ineligible to claim this relief, else input a integer from 0." promptTitle="Item 14b(i)" prompt="Input the number of child._x000a__x000a_By selecting this relief, you will not be eligible to claim relief of Item F14b(ii)._x000a__x000a_If you have already claimed relief of Item F14b(ii), you will not be eligible to claim this relief." sqref="D138" xr:uid="{C40F2F4B-308D-4FDC-91F4-4A1E138036BE}">
       <formula1>AND(OR(D142="",D142=0), D138&gt;=0, INT(D138)=D138)</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Data or Amount" error="The input data or amount is invalid. _x000a__x000a_Please input an integer from 0 to 250 only." promptTitle="Item F18" prompt="Input a postive integer from 0 to 250." sqref="D215:D218" xr:uid="{6B3CA021-B44D-4555-83CC-D39A799FE2DA}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Data or Amount" error="The input data or amount is invalid. _x000a__x000a_Please input an integer from 0 to 250 only." promptTitle="Item F18" prompt="Input a postive integer from 0 to 250." sqref="D215:D216" xr:uid="{6B3CA021-B44D-4555-83CC-D39A799FE2DA}">
       <formula1>0</formula1>
       <formula2>250</formula2>
     </dataValidation>
@@ -8534,6 +8534,10 @@
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Data or Amount" error="The input data or amount is invalid. _x000a__x000a_Please input an integer from 0 to 250 only." promptTitle="Item F18" prompt="Input a postive integer from 0 to 350." sqref="D217:D218" xr:uid="{03F5E266-46A0-4AC6-A144-04FE17B05583}">
+      <formula1>0</formula1>
+      <formula2>350</formula2>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E41" r:id="rId1" xr:uid="{0A00DF98-B175-4727-A964-9E786BBE279D}"/>
@@ -8551,10 +8555,10 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C5" sqref="C5:C17"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>